<commit_message>
Nose que es pero no lo commite
</commit_message>
<xml_diff>
--- a/Calculos.xlsx
+++ b/Calculos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40CDFA1-78D2-4770-9E58-449C95FFBB5B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B1C053-18A3-4D12-988E-A73B35799421}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7636,7 +7636,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>First</c:v>
+            <c:v>LS8</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
@@ -7968,7 +7968,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Best</c:v>
+            <c:v>LS4</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
@@ -8608,7 +8608,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>ILS</c:v>
+            <c:v>ILS4</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
@@ -9237,7 +9237,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Best</c:v>
+            <c:v>LS4</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd">
@@ -14901,8 +14901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BQ363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO250" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="BY269" sqref="BY269"/>
+    <sheetView tabSelected="1" topLeftCell="BL247" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="CC260" sqref="CC260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>